<commit_message>
Adición del índice RONI y corrección en el clasificador para los indices NIÑO#
</commit_message>
<xml_diff>
--- a/IMT/IMT_2025_Actualizado2.xlsx
+++ b/IMT/IMT_2025_Actualizado2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\home\chrisbermudezr\Indices_Climaticos\IMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43A45461-19A6-4672-8699-C792AA75146B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170D2435-FE62-4B86-8001-59500690C219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="37900" xr2:uid="{124AE8C5-2E57-40E8-8D65-3CCB56C3FE50}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>date</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>No aplicable</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Fase fría neutra</t>
+  </si>
+  <si>
+    <t>Neutro</t>
+  </si>
+  <si>
+    <t>Condiciones Neutras</t>
   </si>
 </sst>
 </file>
@@ -557,9 +569,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -935,15 +948,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B698C7F-794A-4ABD-9786-ED36FD83AFE7}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -980,10 +1002,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="B2">
-        <v>-1.7894000000000001</v>
+        <v>-1.1153</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -995,18 +1017,50 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B3">
+        <v>-1.355</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>